<commit_message>
Assigned priority values to risks
</commit_message>
<xml_diff>
--- a/Managing Risk/Raid Log.xlsx
+++ b/Managing Risk/Raid Log.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29512"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29426"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{0072F9BE-AF80-4190-9352-A9DD98577590}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="20" documentId="8_{0072F9BE-AF80-4190-9352-A9DD98577590}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B950B52C-6787-451F-B9CF-458E1A44E9FF}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Log" sheetId="1" r:id="rId1"/>
@@ -231,7 +231,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$-409]d\-mmm\-yy;@"/>
   </numFmts>
-  <fonts count="26">
+  <fonts count="26" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -406,8 +406,9 @@
     <font>
       <sz val="9"/>
       <color rgb="FF000000"/>
-      <name val="Aptos Narrow"/>
+      <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="11">
@@ -685,7 +686,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="66">
+  <cellXfs count="67">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
@@ -847,7 +848,6 @@
     <xf numFmtId="9" fontId="24" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -865,6 +865,13 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1254,11 +1261,11 @@
   </sheetPr>
   <dimension ref="A1:Q249"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A6" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="R8" sqref="R8"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12"/>
+  <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="2.7109375" style="4" customWidth="1"/>
     <col min="2" max="2" width="16.7109375" style="4" customWidth="1"/>
@@ -1588,7 +1595,7 @@
     <col min="16383" max="16384" width="8.85546875" style="4" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="25.9">
+    <row r="1" spans="1:17" ht="26.25" x14ac:dyDescent="0.2">
       <c r="A1" s="3"/>
       <c r="B1" s="42" t="s">
         <v>0</v>
@@ -1613,7 +1620,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:17" s="5" customFormat="1" ht="6" customHeight="1">
+    <row r="2" spans="1:17" s="5" customFormat="1" ht="6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C2" s="6"/>
       <c r="E2" s="7"/>
       <c r="G2" s="6"/>
@@ -1646,7 +1653,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:17" s="5" customFormat="1" ht="18" customHeight="1">
+    <row r="3" spans="1:17" s="5" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="6" t="s">
         <v>8</v>
       </c>
@@ -1693,7 +1700,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:17" s="5" customFormat="1" ht="6" customHeight="1">
+    <row r="4" spans="1:17" s="5" customFormat="1" ht="6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B4" s="8"/>
       <c r="C4" s="9"/>
       <c r="D4" s="8"/>
@@ -1727,7 +1734,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:17" s="5" customFormat="1" ht="18" customHeight="1">
+    <row r="5" spans="1:17" s="5" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B5" s="4"/>
       <c r="C5" s="36" t="s">
         <v>15</v>
@@ -1736,13 +1743,13 @@
         <v>16</v>
       </c>
       <c r="E5" s="30">
-        <v>45952</v>
+        <v>46001</v>
       </c>
       <c r="F5" s="6" t="s">
         <v>17</v>
       </c>
       <c r="G5" s="1">
-        <v>1.2</v>
+        <v>1.3</v>
       </c>
       <c r="J5" s="10"/>
       <c r="K5" s="31" t="s">
@@ -1773,7 +1780,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:17" s="5" customFormat="1" ht="15" customHeight="1" thickBot="1">
+    <row r="6" spans="1:17" s="5" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B6" s="38" t="s">
         <v>19</v>
       </c>
@@ -1804,7 +1811,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:17" ht="6" customHeight="1" thickTop="1">
+    <row r="7" spans="1:17" ht="6" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A7" s="13"/>
       <c r="B7" s="14"/>
       <c r="C7" s="14"/>
@@ -1814,7 +1821,7 @@
       <c r="G7" s="14"/>
       <c r="H7" s="15"/>
     </row>
-    <row r="8" spans="1:17" s="17" customFormat="1" ht="24" customHeight="1">
+    <row r="8" spans="1:17" s="17" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="16"/>
       <c r="B8" s="51" t="s">
         <v>22</v>
@@ -1846,14 +1853,14 @@
       <c r="P8" s="4"/>
       <c r="Q8" s="4"/>
     </row>
-    <row r="9" spans="1:17" ht="18" customHeight="1">
+    <row r="9" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="18">
         <v>1</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C9" s="59" t="s">
+      <c r="C9" s="66" t="s">
         <v>29</v>
       </c>
       <c r="D9" s="56" t="s">
@@ -1865,7 +1872,9 @@
       <c r="F9" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="G9" s="2"/>
+      <c r="G9" s="2">
+        <v>10</v>
+      </c>
       <c r="H9" s="35" t="s">
         <v>31</v>
       </c>
@@ -1873,14 +1882,14 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:17" ht="18" customHeight="1">
+    <row r="10" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="18">
         <v>2</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C10" s="59" t="s">
+      <c r="C10" s="66" t="s">
         <v>32</v>
       </c>
       <c r="D10" s="56" t="s">
@@ -1892,7 +1901,9 @@
       <c r="F10" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="G10" s="2"/>
+      <c r="G10" s="2">
+        <v>2</v>
+      </c>
       <c r="H10" s="35" t="s">
         <v>31</v>
       </c>
@@ -1900,14 +1911,14 @@
         <v>13</v>
       </c>
     </row>
-    <row r="11" spans="1:17" ht="18" customHeight="1">
+    <row r="11" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="18">
         <v>3</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C11" s="59" t="s">
+      <c r="C11" s="66" t="s">
         <v>34</v>
       </c>
       <c r="D11" s="56" t="s">
@@ -1919,7 +1930,9 @@
       <c r="F11" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="G11" s="2"/>
+      <c r="G11" s="2">
+        <v>11</v>
+      </c>
       <c r="H11" s="35" t="s">
         <v>31</v>
       </c>
@@ -1927,14 +1940,14 @@
         <v>14</v>
       </c>
     </row>
-    <row r="12" spans="1:17" ht="18" customHeight="1">
+    <row r="12" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="18">
         <v>4</v>
       </c>
       <c r="B12" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C12" s="59" t="s">
+      <c r="C12" s="66" t="s">
         <v>36</v>
       </c>
       <c r="D12" s="56" t="s">
@@ -1946,7 +1959,9 @@
       <c r="F12" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="G12" s="2"/>
+      <c r="G12" s="2">
+        <v>3</v>
+      </c>
       <c r="H12" s="35" t="s">
         <v>31</v>
       </c>
@@ -1954,14 +1969,14 @@
         <v>18</v>
       </c>
     </row>
-    <row r="13" spans="1:17" ht="18" customHeight="1">
+    <row r="13" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="18">
         <v>5</v>
       </c>
       <c r="B13" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C13" s="59" t="s">
+      <c r="C13" s="66" t="s">
         <v>37</v>
       </c>
       <c r="D13" s="56" t="s">
@@ -1973,20 +1988,22 @@
       <c r="F13" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="G13" s="2"/>
+      <c r="G13" s="2">
+        <v>4</v>
+      </c>
       <c r="H13" s="35" t="s">
         <v>31</v>
       </c>
       <c r="I13" s="58"/>
     </row>
-    <row r="14" spans="1:17" ht="18" customHeight="1">
+    <row r="14" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="18">
         <v>6</v>
       </c>
       <c r="B14" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C14" s="59" t="s">
+      <c r="C14" s="66" t="s">
         <v>38</v>
       </c>
       <c r="D14" s="56" t="s">
@@ -1998,7 +2015,9 @@
       <c r="F14" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="G14" s="2"/>
+      <c r="G14" s="2">
+        <v>12</v>
+      </c>
       <c r="H14" s="35" t="s">
         <v>31</v>
       </c>
@@ -2006,14 +2025,14 @@
         <v>31</v>
       </c>
     </row>
-    <row r="15" spans="1:17" ht="18" customHeight="1">
+    <row r="15" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="18">
         <v>7</v>
       </c>
       <c r="B15" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C15" s="59" t="s">
+      <c r="C15" s="66" t="s">
         <v>40</v>
       </c>
       <c r="D15" s="56" t="s">
@@ -2025,7 +2044,9 @@
       <c r="F15" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="G15" s="2"/>
+      <c r="G15" s="2">
+        <v>1</v>
+      </c>
       <c r="H15" s="35" t="s">
         <v>31</v>
       </c>
@@ -2033,14 +2054,14 @@
         <v>41</v>
       </c>
     </row>
-    <row r="16" spans="1:17" ht="18" customHeight="1">
+    <row r="16" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="18">
         <v>8</v>
       </c>
       <c r="B16" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C16" s="59" t="s">
+      <c r="C16" s="66" t="s">
         <v>42</v>
       </c>
       <c r="D16" s="56" t="s">
@@ -2052,20 +2073,22 @@
       <c r="F16" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="G16" s="2"/>
+      <c r="G16" s="2">
+        <v>5</v>
+      </c>
       <c r="H16" s="35" t="s">
         <v>31</v>
       </c>
       <c r="I16" s="58"/>
     </row>
-    <row r="17" spans="1:9" ht="18" customHeight="1">
+    <row r="17" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="18">
         <v>9</v>
       </c>
       <c r="B17" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C17" s="59" t="s">
+      <c r="C17" s="66" t="s">
         <v>43</v>
       </c>
       <c r="D17" s="56" t="s">
@@ -2077,7 +2100,9 @@
       <c r="F17" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="G17" s="2"/>
+      <c r="G17" s="2">
+        <v>6</v>
+      </c>
       <c r="H17" s="35" t="s">
         <v>31</v>
       </c>
@@ -2085,14 +2110,14 @@
         <v>2</v>
       </c>
     </row>
-    <row r="18" spans="1:9" ht="18" customHeight="1">
+    <row r="18" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="18">
         <v>10</v>
       </c>
       <c r="B18" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C18" s="59" t="s">
+      <c r="C18" s="66" t="s">
         <v>45</v>
       </c>
       <c r="D18" s="56" t="s">
@@ -2104,7 +2129,9 @@
       <c r="F18" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="G18" s="2"/>
+      <c r="G18" s="2">
+        <v>13</v>
+      </c>
       <c r="H18" s="35" t="s">
         <v>31</v>
       </c>
@@ -2112,14 +2139,14 @@
         <v>3</v>
       </c>
     </row>
-    <row r="19" spans="1:9" ht="18" customHeight="1">
+    <row r="19" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="18">
         <v>11</v>
       </c>
       <c r="B19" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C19" s="59" t="s">
+      <c r="C19" s="66" t="s">
         <v>46</v>
       </c>
       <c r="D19" s="56" t="s">
@@ -2131,7 +2158,9 @@
       <c r="F19" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G19" s="2"/>
+      <c r="G19" s="2">
+        <v>15</v>
+      </c>
       <c r="H19" s="35" t="s">
         <v>31</v>
       </c>
@@ -2139,14 +2168,14 @@
         <v>4</v>
       </c>
     </row>
-    <row r="20" spans="1:9" ht="18" customHeight="1">
+    <row r="20" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="18">
         <v>12</v>
       </c>
       <c r="B20" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="C20" s="37" t="s">
+      <c r="C20" s="65" t="s">
         <v>47</v>
       </c>
       <c r="D20" s="56" t="s">
@@ -2158,7 +2187,9 @@
       <c r="F20" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="G20" s="2"/>
+      <c r="G20" s="2">
+        <v>7</v>
+      </c>
       <c r="H20" s="35" t="s">
         <v>31</v>
       </c>
@@ -2166,14 +2197,14 @@
         <v>5</v>
       </c>
     </row>
-    <row r="21" spans="1:9" ht="18" customHeight="1">
+    <row r="21" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="18">
         <v>13</v>
       </c>
       <c r="B21" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="C21" s="37" t="s">
+      <c r="C21" s="65" t="s">
         <v>48</v>
       </c>
       <c r="D21" s="56" t="s">
@@ -2185,7 +2216,9 @@
       <c r="F21" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="G21" s="2"/>
+      <c r="G21" s="2">
+        <v>8</v>
+      </c>
       <c r="H21" s="35" t="s">
         <v>31</v>
       </c>
@@ -2193,14 +2226,14 @@
         <v>6</v>
       </c>
     </row>
-    <row r="22" spans="1:9" ht="18" customHeight="1">
+    <row r="22" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="18">
         <v>14</v>
       </c>
       <c r="B22" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C22" s="37" t="s">
+      <c r="C22" s="65" t="s">
         <v>49</v>
       </c>
       <c r="D22" s="56" t="s">
@@ -2212,20 +2245,22 @@
       <c r="F22" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="G22" s="2"/>
+      <c r="G22" s="2">
+        <v>14</v>
+      </c>
       <c r="H22" s="35" t="s">
         <v>31</v>
       </c>
       <c r="I22" s="58"/>
     </row>
-    <row r="23" spans="1:9" ht="18" customHeight="1">
+    <row r="23" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="18">
         <v>15</v>
       </c>
       <c r="B23" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C23" s="37" t="s">
+      <c r="C23" s="65" t="s">
         <v>50</v>
       </c>
       <c r="D23" s="56" t="s">
@@ -2237,13 +2272,15 @@
       <c r="F23" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="G23" s="2"/>
+      <c r="G23" s="2">
+        <v>9</v>
+      </c>
       <c r="H23" s="35" t="s">
         <v>31</v>
       </c>
       <c r="I23" s="58"/>
     </row>
-    <row r="24" spans="1:9" ht="18" customHeight="1">
+    <row r="24" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="18">
         <v>16</v>
       </c>
@@ -2256,7 +2293,7 @@
       <c r="H24" s="35"/>
       <c r="I24" s="58"/>
     </row>
-    <row r="25" spans="1:9" ht="18" customHeight="1">
+    <row r="25" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="18">
         <v>17</v>
       </c>
@@ -2269,7 +2306,7 @@
       <c r="H25" s="35"/>
       <c r="I25" s="58"/>
     </row>
-    <row r="26" spans="1:9" ht="18" customHeight="1">
+    <row r="26" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="18">
         <v>18</v>
       </c>
@@ -2282,7 +2319,7 @@
       <c r="H26" s="35"/>
       <c r="I26" s="58"/>
     </row>
-    <row r="27" spans="1:9" ht="18" customHeight="1">
+    <row r="27" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="18">
         <v>19</v>
       </c>
@@ -2295,7 +2332,7 @@
       <c r="H27" s="35"/>
       <c r="I27" s="58"/>
     </row>
-    <row r="28" spans="1:9" ht="18" customHeight="1">
+    <row r="28" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="18">
         <v>20</v>
       </c>
@@ -2308,7 +2345,7 @@
       <c r="H28" s="35"/>
       <c r="I28" s="58"/>
     </row>
-    <row r="29" spans="1:9" ht="18" customHeight="1">
+    <row r="29" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="18">
         <v>21</v>
       </c>
@@ -2321,7 +2358,7 @@
       <c r="H29" s="35"/>
       <c r="I29" s="58"/>
     </row>
-    <row r="30" spans="1:9" ht="18" customHeight="1">
+    <row r="30" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="18">
         <v>22</v>
       </c>
@@ -2334,7 +2371,7 @@
       <c r="H30" s="35"/>
       <c r="I30" s="58"/>
     </row>
-    <row r="31" spans="1:9" ht="18" customHeight="1">
+    <row r="31" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="18">
         <v>23</v>
       </c>
@@ -2347,7 +2384,7 @@
       <c r="H31" s="35"/>
       <c r="I31" s="58"/>
     </row>
-    <row r="32" spans="1:9" ht="18" customHeight="1">
+    <row r="32" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="18">
         <v>24</v>
       </c>
@@ -2360,7 +2397,7 @@
       <c r="H32" s="35"/>
       <c r="I32" s="58"/>
     </row>
-    <row r="33" spans="1:8" ht="6" customHeight="1" thickBot="1">
+    <row r="33" spans="1:8" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A33" s="13"/>
       <c r="B33" s="19"/>
       <c r="C33" s="19"/>
@@ -2370,241 +2407,241 @@
       <c r="G33" s="19"/>
       <c r="H33" s="20"/>
     </row>
-    <row r="34" spans="1:8" ht="14.45" customHeight="1" thickTop="1"/>
-    <row r="35" spans="1:8" ht="14.45" customHeight="1">
-      <c r="B35" s="60" t="s">
+    <row r="34" spans="1:8" ht="14.45" customHeight="1" thickTop="1" x14ac:dyDescent="0.2"/>
+    <row r="35" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B35" s="59" t="s">
         <v>51</v>
       </c>
-      <c r="C35" s="60"/>
-      <c r="D35" s="60"/>
-      <c r="E35" s="60"/>
-      <c r="F35" s="60"/>
-      <c r="G35" s="60"/>
-      <c r="H35" s="60"/>
-    </row>
-    <row r="36" spans="1:8" ht="12.75" customHeight="1"/>
-    <row r="37" spans="1:8" ht="12.75" customHeight="1">
+      <c r="C35" s="59"/>
+      <c r="D35" s="59"/>
+      <c r="E35" s="59"/>
+      <c r="F35" s="59"/>
+      <c r="G35" s="59"/>
+      <c r="H35" s="59"/>
+    </row>
+    <row r="36" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="37" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B37" s="39" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="38" spans="1:8" ht="12.75" customHeight="1">
+    <row r="38" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B38" s="40" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="39" spans="1:8" ht="12.75" customHeight="1">
+    <row r="39" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B39" s="40" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="40" spans="1:8" ht="12.75" customHeight="1">
+    <row r="40" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B40" s="40" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="41" spans="1:8" ht="12.75" customHeight="1"/>
-    <row r="42" spans="1:8" ht="12.75" customHeight="1"/>
-    <row r="43" spans="1:8" ht="12.75" customHeight="1"/>
-    <row r="44" spans="1:8" ht="12.75" customHeight="1"/>
-    <row r="45" spans="1:8" ht="12.75" customHeight="1"/>
-    <row r="46" spans="1:8" ht="12.75" customHeight="1"/>
-    <row r="47" spans="1:8" ht="12.75" customHeight="1"/>
-    <row r="48" spans="1:8" ht="12.75" customHeight="1"/>
-    <row r="49" ht="12.75" customHeight="1"/>
-    <row r="50" ht="12.75" customHeight="1"/>
-    <row r="51" ht="12.75" customHeight="1"/>
-    <row r="52" ht="12.75" customHeight="1"/>
-    <row r="53" ht="12.75" customHeight="1"/>
-    <row r="54" ht="12.75" customHeight="1"/>
-    <row r="55" ht="12.75" customHeight="1"/>
-    <row r="56" ht="12.75" customHeight="1"/>
-    <row r="57" ht="12.75" customHeight="1"/>
-    <row r="58" ht="12.75" customHeight="1"/>
-    <row r="59" ht="12.75" customHeight="1"/>
-    <row r="60" ht="12.75" customHeight="1"/>
-    <row r="61" ht="12.75" customHeight="1"/>
-    <row r="62" ht="12.75" customHeight="1"/>
-    <row r="63" ht="12.75" customHeight="1"/>
-    <row r="64" ht="12.75" customHeight="1"/>
-    <row r="65" ht="12.75" customHeight="1"/>
-    <row r="66" ht="12.75" customHeight="1"/>
-    <row r="67" ht="12.75" customHeight="1"/>
-    <row r="68" ht="12.75" customHeight="1"/>
-    <row r="69" ht="12.75" customHeight="1"/>
-    <row r="70" ht="12.75" customHeight="1"/>
-    <row r="71" ht="12.75" customHeight="1"/>
-    <row r="72" ht="12.75" customHeight="1"/>
-    <row r="73" ht="12.75" customHeight="1"/>
-    <row r="81" s="4" customFormat="1"/>
-    <row r="82" s="4" customFormat="1"/>
-    <row r="83" s="4" customFormat="1"/>
-    <row r="84" s="4" customFormat="1"/>
-    <row r="85" s="4" customFormat="1"/>
-    <row r="86" s="4" customFormat="1"/>
-    <row r="87" s="4" customFormat="1"/>
-    <row r="88" s="4" customFormat="1"/>
-    <row r="89" s="4" customFormat="1"/>
-    <row r="90" s="4" customFormat="1"/>
-    <row r="91" s="4" customFormat="1"/>
-    <row r="92" s="4" customFormat="1"/>
-    <row r="93" s="4" customFormat="1"/>
-    <row r="94" s="4" customFormat="1"/>
-    <row r="95" s="4" customFormat="1"/>
-    <row r="96" s="4" customFormat="1"/>
-    <row r="97" s="4" customFormat="1"/>
-    <row r="98" s="4" customFormat="1"/>
-    <row r="99" s="4" customFormat="1"/>
-    <row r="100" s="4" customFormat="1"/>
-    <row r="101" s="4" customFormat="1"/>
-    <row r="102" s="4" customFormat="1"/>
-    <row r="103" s="4" customFormat="1"/>
-    <row r="104" s="4" customFormat="1"/>
-    <row r="105" s="4" customFormat="1"/>
-    <row r="106" s="4" customFormat="1"/>
-    <row r="107" s="4" customFormat="1"/>
-    <row r="108" s="4" customFormat="1"/>
-    <row r="109" s="4" customFormat="1"/>
-    <row r="110" s="4" customFormat="1"/>
-    <row r="111" s="4" customFormat="1"/>
-    <row r="112" s="4" customFormat="1"/>
-    <row r="113" s="4" customFormat="1"/>
-    <row r="114" s="4" customFormat="1"/>
-    <row r="115" s="4" customFormat="1"/>
-    <row r="116" s="4" customFormat="1"/>
-    <row r="117" s="4" customFormat="1"/>
-    <row r="118" s="4" customFormat="1"/>
-    <row r="119" s="4" customFormat="1"/>
-    <row r="120" s="4" customFormat="1"/>
-    <row r="121" s="4" customFormat="1"/>
-    <row r="122" s="4" customFormat="1"/>
-    <row r="123" s="4" customFormat="1"/>
-    <row r="124" s="4" customFormat="1"/>
-    <row r="125" s="4" customFormat="1"/>
-    <row r="126" s="4" customFormat="1"/>
-    <row r="127" s="4" customFormat="1"/>
-    <row r="128" s="4" customFormat="1"/>
-    <row r="129" s="4" customFormat="1"/>
-    <row r="130" s="4" customFormat="1"/>
-    <row r="131" s="4" customFormat="1"/>
-    <row r="132" s="4" customFormat="1"/>
-    <row r="133" s="4" customFormat="1"/>
-    <row r="134" s="4" customFormat="1"/>
-    <row r="135" s="4" customFormat="1"/>
-    <row r="136" s="4" customFormat="1"/>
-    <row r="137" s="4" customFormat="1"/>
-    <row r="138" s="4" customFormat="1"/>
-    <row r="139" s="4" customFormat="1"/>
-    <row r="140" s="4" customFormat="1"/>
-    <row r="141" s="4" customFormat="1"/>
-    <row r="142" s="4" customFormat="1"/>
-    <row r="143" s="4" customFormat="1"/>
-    <row r="144" s="4" customFormat="1"/>
-    <row r="145" s="4" customFormat="1"/>
-    <row r="146" s="4" customFormat="1"/>
-    <row r="147" s="4" customFormat="1"/>
-    <row r="148" s="4" customFormat="1"/>
-    <row r="149" s="4" customFormat="1"/>
-    <row r="150" s="4" customFormat="1"/>
-    <row r="151" s="4" customFormat="1"/>
-    <row r="152" s="4" customFormat="1"/>
-    <row r="153" s="4" customFormat="1"/>
-    <row r="154" s="4" customFormat="1"/>
-    <row r="155" s="4" customFormat="1"/>
-    <row r="156" s="4" customFormat="1"/>
-    <row r="157" s="4" customFormat="1"/>
-    <row r="158" s="4" customFormat="1"/>
-    <row r="159" s="4" customFormat="1"/>
-    <row r="160" s="4" customFormat="1"/>
-    <row r="161" s="4" customFormat="1"/>
-    <row r="162" s="4" customFormat="1"/>
-    <row r="163" s="4" customFormat="1"/>
-    <row r="164" s="4" customFormat="1"/>
-    <row r="165" s="4" customFormat="1"/>
-    <row r="166" s="4" customFormat="1"/>
-    <row r="167" s="4" customFormat="1"/>
-    <row r="168" s="4" customFormat="1"/>
-    <row r="169" s="4" customFormat="1"/>
-    <row r="170" s="4" customFormat="1"/>
-    <row r="171" s="4" customFormat="1"/>
-    <row r="172" s="4" customFormat="1"/>
-    <row r="173" s="4" customFormat="1"/>
-    <row r="174" s="4" customFormat="1"/>
-    <row r="175" s="4" customFormat="1"/>
-    <row r="176" s="4" customFormat="1"/>
-    <row r="177" s="4" customFormat="1"/>
-    <row r="178" s="4" customFormat="1"/>
-    <row r="179" s="4" customFormat="1"/>
-    <row r="180" s="4" customFormat="1"/>
-    <row r="181" s="4" customFormat="1"/>
-    <row r="182" s="4" customFormat="1"/>
-    <row r="183" s="4" customFormat="1"/>
-    <row r="184" s="4" customFormat="1"/>
-    <row r="185" s="4" customFormat="1"/>
-    <row r="186" s="4" customFormat="1"/>
-    <row r="187" s="4" customFormat="1"/>
-    <row r="188" s="4" customFormat="1"/>
-    <row r="189" s="4" customFormat="1"/>
-    <row r="190" s="4" customFormat="1"/>
-    <row r="191" s="4" customFormat="1"/>
-    <row r="192" s="4" customFormat="1"/>
-    <row r="193" s="4" customFormat="1"/>
-    <row r="194" s="4" customFormat="1"/>
-    <row r="195" s="4" customFormat="1"/>
-    <row r="196" s="4" customFormat="1"/>
-    <row r="197" s="4" customFormat="1"/>
-    <row r="198" s="4" customFormat="1"/>
-    <row r="199" s="4" customFormat="1"/>
-    <row r="200" s="4" customFormat="1"/>
-    <row r="201" s="4" customFormat="1"/>
-    <row r="202" s="4" customFormat="1"/>
-    <row r="203" s="4" customFormat="1"/>
-    <row r="204" s="4" customFormat="1"/>
-    <row r="205" s="4" customFormat="1"/>
-    <row r="206" s="4" customFormat="1"/>
-    <row r="207" s="4" customFormat="1"/>
-    <row r="208" s="4" customFormat="1"/>
-    <row r="209" s="4" customFormat="1"/>
-    <row r="210" s="4" customFormat="1"/>
-    <row r="211" s="4" customFormat="1"/>
-    <row r="212" s="4" customFormat="1"/>
-    <row r="213" s="4" customFormat="1"/>
-    <row r="214" s="4" customFormat="1"/>
-    <row r="215" s="4" customFormat="1"/>
-    <row r="216" s="4" customFormat="1"/>
-    <row r="217" s="4" customFormat="1"/>
-    <row r="218" s="4" customFormat="1"/>
-    <row r="219" s="4" customFormat="1"/>
-    <row r="220" s="4" customFormat="1"/>
-    <row r="221" s="4" customFormat="1"/>
-    <row r="222" s="4" customFormat="1"/>
-    <row r="223" s="4" customFormat="1"/>
-    <row r="224" s="4" customFormat="1"/>
-    <row r="225" s="4" customFormat="1"/>
-    <row r="226" s="4" customFormat="1"/>
-    <row r="227" s="4" customFormat="1"/>
-    <row r="228" s="4" customFormat="1"/>
-    <row r="229" s="4" customFormat="1"/>
-    <row r="230" s="4" customFormat="1"/>
-    <row r="231" s="4" customFormat="1"/>
-    <row r="232" s="4" customFormat="1"/>
-    <row r="233" s="4" customFormat="1"/>
-    <row r="234" s="4" customFormat="1"/>
-    <row r="235" s="4" customFormat="1"/>
-    <row r="236" s="4" customFormat="1"/>
-    <row r="237" s="4" customFormat="1"/>
-    <row r="238" s="4" customFormat="1"/>
-    <row r="239" s="4" customFormat="1"/>
-    <row r="240" s="4" customFormat="1"/>
-    <row r="241" s="4" customFormat="1"/>
-    <row r="242" s="4" customFormat="1"/>
-    <row r="243" s="4" customFormat="1"/>
-    <row r="244" s="4" customFormat="1"/>
-    <row r="245" s="4" customFormat="1"/>
-    <row r="246" s="4" customFormat="1"/>
-    <row r="247" s="4" customFormat="1"/>
-    <row r="248" s="4" customFormat="1"/>
-    <row r="249" s="4" customFormat="1"/>
+    <row r="41" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="42" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="43" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="44" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="45" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="46" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="47" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="48" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="49" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="50" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="51" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="52" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="53" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="54" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="55" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="56" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="57" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="58" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="59" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="60" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="61" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="62" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="63" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="64" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="65" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="66" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="67" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="68" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="69" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="70" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="71" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="72" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="73" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="81" s="4" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="82" s="4" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="83" s="4" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="84" s="4" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="85" s="4" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="86" s="4" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="87" s="4" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="88" s="4" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="89" s="4" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="90" s="4" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="91" s="4" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="92" s="4" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="93" s="4" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="94" s="4" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="95" s="4" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="96" s="4" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="97" s="4" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="98" s="4" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="99" s="4" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="100" s="4" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="101" s="4" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="102" s="4" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="103" s="4" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="104" s="4" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="105" s="4" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="106" s="4" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="107" s="4" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="108" s="4" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="109" s="4" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="110" s="4" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="111" s="4" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="112" s="4" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="113" s="4" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="114" s="4" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="115" s="4" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="116" s="4" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="117" s="4" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="118" s="4" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="119" s="4" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="120" s="4" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="121" s="4" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="122" s="4" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="123" s="4" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="124" s="4" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="125" s="4" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="126" s="4" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="127" s="4" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="128" s="4" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="129" s="4" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="130" s="4" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="131" s="4" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="132" s="4" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="133" s="4" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="134" s="4" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="135" s="4" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="136" s="4" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="137" s="4" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="138" s="4" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="139" s="4" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="140" s="4" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="141" s="4" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="142" s="4" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="143" s="4" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="144" s="4" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="145" s="4" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="146" s="4" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="147" s="4" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="148" s="4" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="149" s="4" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="150" s="4" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="151" s="4" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="152" s="4" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="153" s="4" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="154" s="4" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="155" s="4" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="156" s="4" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="157" s="4" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="158" s="4" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="159" s="4" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="160" s="4" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="161" s="4" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="162" s="4" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="163" s="4" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="164" s="4" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="165" s="4" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="166" s="4" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="167" s="4" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="168" s="4" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="169" s="4" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="170" s="4" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="171" s="4" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="172" s="4" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="173" s="4" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="174" s="4" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="175" s="4" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="176" s="4" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="177" s="4" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="178" s="4" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="179" s="4" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="180" s="4" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="181" s="4" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="182" s="4" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="183" s="4" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="184" s="4" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="185" s="4" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="186" s="4" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="187" s="4" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="188" s="4" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="189" s="4" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="190" s="4" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="191" s="4" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="192" s="4" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="193" s="4" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="194" s="4" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="195" s="4" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="196" s="4" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="197" s="4" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="198" s="4" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="199" s="4" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="200" s="4" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="201" s="4" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="202" s="4" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="203" s="4" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="204" s="4" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="205" s="4" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="206" s="4" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="207" s="4" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="208" s="4" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="209" s="4" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="210" s="4" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="211" s="4" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="212" s="4" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="213" s="4" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="214" s="4" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="215" s="4" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="216" s="4" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="217" s="4" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="218" s="4" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="219" s="4" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="220" s="4" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="221" s="4" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="222" s="4" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="223" s="4" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="224" s="4" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="225" s="4" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="226" s="4" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="227" s="4" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="228" s="4" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="229" s="4" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="230" s="4" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="231" s="4" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="232" s="4" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="233" s="4" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="234" s="4" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="235" s="4" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="236" s="4" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="237" s="4" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="238" s="4" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="239" s="4" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="240" s="4" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="241" s="4" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="242" s="4" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="243" s="4" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="244" s="4" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="245" s="4" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="246" s="4" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="247" s="4" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="248" s="4" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="249" s="4" customFormat="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="B35:H35"/>
@@ -2668,7 +2705,7 @@
   <sheetViews>
     <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="2.7109375" style="7" customWidth="1"/>
     <col min="2" max="2" width="3.7109375" style="7" customWidth="1"/>
@@ -3001,7 +3038,7 @@
     <col min="16139" max="16384" width="9.140625" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="25.9">
+    <row r="1" spans="1:15" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A1" s="21"/>
       <c r="B1" s="42" t="s">
         <v>56</v>
@@ -3009,20 +3046,20 @@
       <c r="J1" s="22"/>
       <c r="M1" s="23"/>
     </row>
-    <row r="2" spans="1:15" ht="6" customHeight="1">
+    <row r="2" spans="1:15" ht="6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C2" s="24"/>
       <c r="G2" s="24"/>
       <c r="I2" s="24"/>
       <c r="K2" s="24"/>
     </row>
-    <row r="3" spans="1:15">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B3" s="25"/>
       <c r="C3" s="26"/>
       <c r="D3" s="25"/>
       <c r="E3" s="26"/>
       <c r="L3" s="24"/>
     </row>
-    <row r="4" spans="1:15">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B4" s="25"/>
       <c r="C4" s="25" t="str">
         <f>Log!B3</f>
@@ -3047,38 +3084,38 @@
       </c>
       <c r="M4" s="28">
         <f>IF(Log!E5=0,"",Log!E5)</f>
-        <v>45952</v>
-      </c>
-    </row>
-    <row r="5" spans="1:15">
+        <v>46001</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B5" s="25"/>
       <c r="C5" s="26"/>
       <c r="D5" s="25"/>
       <c r="E5" s="26"/>
       <c r="L5" s="24"/>
     </row>
-    <row r="6" spans="1:15" ht="24" customHeight="1">
+    <row r="6" spans="1:15" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="25"/>
-      <c r="C6" s="62" t="s">
+      <c r="C6" s="61" t="s">
         <v>57</v>
       </c>
-      <c r="D6" s="63"/>
+      <c r="D6" s="62"/>
       <c r="E6" s="26"/>
-      <c r="F6" s="62" t="s">
+      <c r="F6" s="61" t="s">
         <v>58</v>
       </c>
-      <c r="G6" s="63"/>
-      <c r="I6" s="62" t="s">
+      <c r="G6" s="62"/>
+      <c r="I6" s="61" t="s">
         <v>59</v>
       </c>
-      <c r="J6" s="63"/>
-      <c r="L6" s="62" t="s">
+      <c r="J6" s="62"/>
+      <c r="L6" s="61" t="s">
         <v>60</v>
       </c>
-      <c r="M6" s="63"/>
-    </row>
-    <row r="7" spans="1:15" ht="12" customHeight="1"/>
-    <row r="8" spans="1:15" ht="24" customHeight="1">
+      <c r="M6" s="62"/>
+    </row>
+    <row r="7" spans="1:15" ht="12" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="8" spans="1:15" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C8" s="43">
         <f>Log!M2</f>
         <v>1</v>
@@ -3112,8 +3149,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:15" ht="12" customHeight="1"/>
-    <row r="10" spans="1:15" ht="24" customHeight="1">
+    <row r="9" spans="1:15" ht="12" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="10" spans="1:15" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C10" s="43">
         <f>Log!N2</f>
         <v>6</v>
@@ -3147,8 +3184,8 @@
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:15" ht="12" customHeight="1"/>
-    <row r="12" spans="1:15" ht="24" customHeight="1">
+    <row r="11" spans="1:15" ht="12" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="12" spans="1:15" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C12" s="43">
         <f>Log!O2</f>
         <v>4</v>
@@ -3182,8 +3219,8 @@
         <v>5</v>
       </c>
     </row>
-    <row r="13" spans="1:15" ht="12" customHeight="1"/>
-    <row r="14" spans="1:15" ht="24" customHeight="1">
+    <row r="13" spans="1:15" ht="12" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="14" spans="1:15" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C14" s="43">
         <f>Log!P2</f>
         <v>0</v>
@@ -3217,8 +3254,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:15" ht="12" customHeight="1"/>
-    <row r="16" spans="1:15" ht="24" customHeight="1">
+    <row r="15" spans="1:15" ht="12" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="16" spans="1:15" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C16" s="43">
         <f>Log!Q2</f>
         <v>0</v>
@@ -3252,124 +3289,124 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="3:15" ht="12" customHeight="1"/>
-    <row r="18" spans="3:15" ht="24" customHeight="1">
-      <c r="C18" s="64">
+    <row r="17" spans="3:15" ht="12" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="18" spans="3:15" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C18" s="63">
         <f>SUM(C8,C10,C12,C14,C16)</f>
         <v>11</v>
       </c>
-      <c r="D18" s="65"/>
-      <c r="F18" s="64">
+      <c r="D18" s="64"/>
+      <c r="F18" s="63">
         <f>SUM(F8,F10,F12,F14,F16)</f>
         <v>2</v>
       </c>
-      <c r="G18" s="65"/>
-      <c r="I18" s="64">
+      <c r="G18" s="64"/>
+      <c r="I18" s="63">
         <f>SUM(I8,I10,I12,I14,I16)</f>
         <v>0</v>
       </c>
-      <c r="J18" s="65"/>
-      <c r="L18" s="64">
+      <c r="J18" s="64"/>
+      <c r="L18" s="63">
         <f>SUM(L8,L10,L12,L14,L16)</f>
         <v>2</v>
       </c>
-      <c r="M18" s="65"/>
+      <c r="M18" s="64"/>
       <c r="O18" s="50">
         <f>SUM(C18,F18,I18,L18)</f>
         <v>15</v>
       </c>
     </row>
-    <row r="21" spans="3:15">
-      <c r="C21" s="61" t="s">
+    <row r="21" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C21" s="60" t="s">
         <v>51</v>
       </c>
-      <c r="D21" s="61"/>
-      <c r="E21" s="61"/>
-      <c r="F21" s="61"/>
-      <c r="G21" s="61"/>
-      <c r="H21" s="61"/>
-      <c r="I21" s="61"/>
-      <c r="J21" s="61"/>
-      <c r="K21" s="61"/>
-      <c r="L21" s="61"/>
-      <c r="M21" s="61"/>
-    </row>
-    <row r="23" spans="3:15">
+      <c r="D21" s="60"/>
+      <c r="E21" s="60"/>
+      <c r="F21" s="60"/>
+      <c r="G21" s="60"/>
+      <c r="H21" s="60"/>
+      <c r="I21" s="60"/>
+      <c r="J21" s="60"/>
+      <c r="K21" s="60"/>
+      <c r="L21" s="60"/>
+      <c r="M21" s="60"/>
+    </row>
+    <row r="23" spans="3:15" x14ac:dyDescent="0.2">
       <c r="C23" s="39" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="24" spans="3:15">
+    <row r="24" spans="3:15" x14ac:dyDescent="0.2">
       <c r="C24" s="40" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="33" s="7" customFormat="1"/>
-    <row r="34" s="7" customFormat="1"/>
-    <row r="35" s="7" customFormat="1"/>
-    <row r="36" s="7" customFormat="1"/>
-    <row r="37" s="7" customFormat="1"/>
-    <row r="38" s="7" customFormat="1"/>
-    <row r="39" s="7" customFormat="1"/>
-    <row r="40" s="7" customFormat="1"/>
-    <row r="41" s="7" customFormat="1"/>
-    <row r="42" s="7" customFormat="1"/>
-    <row r="43" s="7" customFormat="1"/>
-    <row r="44" s="7" customFormat="1"/>
-    <row r="45" s="7" customFormat="1"/>
-    <row r="46" s="7" customFormat="1"/>
-    <row r="47" s="7" customFormat="1"/>
-    <row r="48" s="7" customFormat="1"/>
-    <row r="49" s="7" customFormat="1"/>
-    <row r="50" s="7" customFormat="1"/>
-    <row r="51" s="7" customFormat="1"/>
-    <row r="52" s="7" customFormat="1"/>
-    <row r="53" s="7" customFormat="1"/>
-    <row r="54" s="7" customFormat="1"/>
-    <row r="55" s="7" customFormat="1"/>
-    <row r="56" s="7" customFormat="1"/>
-    <row r="57" s="7" customFormat="1"/>
-    <row r="58" s="7" customFormat="1"/>
-    <row r="59" s="7" customFormat="1"/>
-    <row r="60" s="7" customFormat="1"/>
-    <row r="61" s="7" customFormat="1"/>
-    <row r="62" s="7" customFormat="1"/>
-    <row r="63" s="7" customFormat="1"/>
-    <row r="64" s="7" customFormat="1"/>
-    <row r="65" s="7" customFormat="1"/>
-    <row r="66" s="7" customFormat="1"/>
-    <row r="67" s="7" customFormat="1"/>
-    <row r="68" s="7" customFormat="1"/>
-    <row r="69" s="7" customFormat="1"/>
-    <row r="70" s="7" customFormat="1"/>
-    <row r="71" s="7" customFormat="1"/>
-    <row r="72" s="7" customFormat="1"/>
-    <row r="73" s="7" customFormat="1"/>
-    <row r="74" s="7" customFormat="1"/>
-    <row r="75" s="7" customFormat="1"/>
-    <row r="76" s="7" customFormat="1"/>
-    <row r="77" s="7" customFormat="1"/>
-    <row r="78" s="7" customFormat="1"/>
-    <row r="79" s="7" customFormat="1"/>
-    <row r="80" s="7" customFormat="1"/>
-    <row r="81" s="7" customFormat="1"/>
-    <row r="82" s="7" customFormat="1"/>
-    <row r="83" s="7" customFormat="1"/>
-    <row r="84" s="7" customFormat="1"/>
-    <row r="85" s="7" customFormat="1"/>
-    <row r="86" s="7" customFormat="1"/>
-    <row r="87" s="7" customFormat="1"/>
-    <row r="88" s="7" customFormat="1"/>
-    <row r="89" s="7" customFormat="1"/>
-    <row r="90" s="7" customFormat="1"/>
-    <row r="91" s="7" customFormat="1"/>
-    <row r="92" s="7" customFormat="1"/>
-    <row r="93" s="7" customFormat="1"/>
-    <row r="94" s="7" customFormat="1"/>
-    <row r="95" s="7" customFormat="1"/>
-    <row r="96" s="7" customFormat="1"/>
-    <row r="97" s="7" customFormat="1"/>
-    <row r="98" s="7" customFormat="1"/>
+    <row r="33" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="34" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="35" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="36" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="37" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="38" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="39" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="40" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="41" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="42" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="43" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="44" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="45" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="46" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="47" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="48" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="49" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="50" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="51" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="52" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="53" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="54" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="55" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="56" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="57" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="58" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="59" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="60" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="61" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="62" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="63" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="64" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="65" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="66" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="67" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="68" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="69" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="70" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="71" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="72" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="73" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="74" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="75" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="76" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="77" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="78" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="79" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="80" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="81" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="82" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="83" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="84" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="85" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="86" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="87" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="88" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="89" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="90" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="91" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="92" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="93" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="94" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="95" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="96" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="97" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="98" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="9">
     <mergeCell ref="C21:M21"/>
@@ -3389,6 +3426,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100D3021E0C4A6E1544B32A3FA7BC9AD69D" ma:contentTypeVersion="11" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="a497b6f1ec41ab02ced7b2da48e752e4">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="c7d1c007-2860-43a4-afa0-acc4aaabe1c7" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="1215ec290e00ad892de77fad199e3ecf" ns3:_="">
     <xsd:import namespace="c7d1c007-2860-43a4-afa0-acc4aaabe1c7"/>
@@ -3576,12 +3619,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -3592,13 +3629,36 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EED8BCEF-1494-4B3A-A1E2-9B55A09493EE}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5A5C0654-B2B0-4112-89BB-7C5532D1D628}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5A5C0654-B2B0-4112-89BB-7C5532D1D628}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EED8BCEF-1494-4B3A-A1E2-9B55A09493EE}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="c7d1c007-2860-43a4-afa0-acc4aaabe1c7"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3E7C8F0C-27B9-43D5-ADEA-34609579A9C0}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3E7C8F0C-27B9-43D5-ADEA-34609579A9C0}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>